<commit_message>
1 task in progress, 1 completed
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_3_SprintBacklog.xlsx
+++ b/TutorGroup_Deliverable_3_SprintBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleitionbendo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleitionbendo/VS Code/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D05FF08D-3A5C-EF4F-B6FE-61A8AFD18735}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6360CFA-B2BC-5F40-914D-C18C1B388660}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2400" yWindow="460" windowWidth="20840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Number</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">                 Responses need to be saved in a database</t>
+  </si>
+  <si>
+    <t>Hunter 100%</t>
+  </si>
+  <si>
+    <t>Klei 100%, front-end done, working on back-end</t>
   </si>
 </sst>
 </file>
@@ -395,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -511,9 +517,11 @@
         <v>3</v>
       </c>
       <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
@@ -595,9 +603,11 @@
         <v>1</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">

</xml_diff>